<commit_message>
Additional ratings to lecture Halls
</commit_message>
<xml_diff>
--- a/LHRating/lectureHallRating.xlsx
+++ b/LHRating/lectureHallRating.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\LHRating\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2BAC0A6-FE61-4B76-967E-6F55C45B73CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3502D293-C06F-4D79-9526-41BEEBBC7E59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D978910E-D27D-4B95-85B6-662EEE754DFA}"/>
   </bookViews>
@@ -710,7 +710,7 @@
   <dimension ref="A1:N50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1415,10 +1415,12 @@
         <f t="shared" ref="L17" si="6">COUNTIF(B15:B61, K17)</f>
         <v>1</v>
       </c>
-      <c r="M17" s="10"/>
+      <c r="M17" s="10">
+        <v>1</v>
+      </c>
       <c r="N17" s="11">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.3">
@@ -1470,16 +1472,22 @@
       <c r="C19" s="3">
         <v>153</v>
       </c>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
+      <c r="D19" s="1">
+        <v>6</v>
+      </c>
+      <c r="E19" s="1">
+        <v>7.75</v>
+      </c>
+      <c r="F19" s="1">
+        <v>5.5</v>
+      </c>
       <c r="G19" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>19.25</v>
       </c>
       <c r="H19" s="8">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.71296296296296291</v>
       </c>
       <c r="I19">
         <v>27</v>
@@ -1974,7 +1982,7 @@
       </c>
       <c r="M31" s="10">
         <f>SUM(M2:M30)</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="N31" s="10"/>
     </row>
@@ -2425,23 +2433,23 @@
       </c>
       <c r="D49" s="6">
         <f>SUM(D2:D48)</f>
-        <v>77.5</v>
+        <v>83.5</v>
       </c>
       <c r="E49" s="6">
         <f>SUM(E2:E48)</f>
-        <v>73.75</v>
+        <v>81.5</v>
       </c>
       <c r="F49" s="6">
         <f>SUM(F2:F48)</f>
-        <v>53</v>
+        <v>58.5</v>
       </c>
       <c r="G49" s="6">
         <f>SUM(G2:G48)</f>
-        <v>204.25</v>
+        <v>223.5</v>
       </c>
       <c r="H49" s="9">
         <f t="shared" si="3"/>
-        <v>0.16095350669818756</v>
+        <v>0.17612293144208038</v>
       </c>
       <c r="I49" s="6">
         <f>SUM(I2:I48)</f>

</xml_diff>